<commit_message>
added all corners and change
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA36"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,6 +581,11 @@
           <t>reference_wval</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>percentage_change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -694,6 +699,9 @@
       <c r="AA2" s="2" t="n">
         <v>0.086892</v>
       </c>
+      <c r="AB2" s="2" t="n">
+        <v>-5.452515766698875</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -807,6 +815,9 @@
       <c r="AA3" s="3" t="n">
         <v>11.50853933618745</v>
       </c>
+      <c r="AB3" s="3" t="n">
+        <v>5.766960179759497</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -916,6 +927,7 @@
       </c>
       <c r="Z4" s="3" t="inlineStr"/>
       <c r="AA4" s="3" t="inlineStr"/>
+      <c r="AB4" s="3" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -1025,6 +1037,7 @@
       </c>
       <c r="Z5" s="3" t="inlineStr"/>
       <c r="AA5" s="3" t="inlineStr"/>
+      <c r="AB5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -1134,6 +1147,7 @@
       </c>
       <c r="Z6" s="3" t="inlineStr"/>
       <c r="AA6" s="3" t="inlineStr"/>
+      <c r="AB6" s="3" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -1243,6 +1257,7 @@
       </c>
       <c r="Z7" s="3" t="inlineStr"/>
       <c r="AA7" s="3" t="inlineStr"/>
+      <c r="AB7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -1352,6 +1367,7 @@
       </c>
       <c r="Z8" s="3" t="inlineStr"/>
       <c r="AA8" s="3" t="inlineStr"/>
+      <c r="AB8" s="3" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -1459,8 +1475,15 @@
       <c r="Y9" s="2" t="n">
         <v>4.3</v>
       </c>
-      <c r="Z9" s="2" t="inlineStr"/>
-      <c r="AA9" s="2" t="inlineStr"/>
+      <c r="Z9" s="2" t="n">
+        <v>0.290291</v>
+      </c>
+      <c r="AA9" s="2" t="n">
+        <v>0.296605</v>
+      </c>
+      <c r="AB9" s="2" t="n">
+        <v>-2.128757101195188</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -1568,8 +1591,15 @@
       <c r="Y10" s="3" t="n">
         <v>-4.101</v>
       </c>
-      <c r="Z10" s="3" t="inlineStr"/>
-      <c r="AA10" s="3" t="inlineStr"/>
+      <c r="Z10" s="3" t="n">
+        <v>3.444819164217974</v>
+      </c>
+      <c r="AA10" s="3" t="n">
+        <v>3.371487331636351</v>
+      </c>
+      <c r="AB10" s="3" t="n">
+        <v>2.175058820287223</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -1679,6 +1709,7 @@
       </c>
       <c r="Z11" s="3" t="inlineStr"/>
       <c r="AA11" s="3" t="inlineStr"/>
+      <c r="AB11" s="3" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
@@ -1788,6 +1819,7 @@
       </c>
       <c r="Z12" s="3" t="inlineStr"/>
       <c r="AA12" s="3" t="inlineStr"/>
+      <c r="AB12" s="3" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
@@ -1897,6 +1929,7 @@
       </c>
       <c r="Z13" s="3" t="inlineStr"/>
       <c r="AA13" s="3" t="inlineStr"/>
+      <c r="AB13" s="3" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
@@ -2006,6 +2039,7 @@
       </c>
       <c r="Z14" s="3" t="inlineStr"/>
       <c r="AA14" s="3" t="inlineStr"/>
+      <c r="AB14" s="3" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -2115,6 +2149,7 @@
       </c>
       <c r="Z15" s="3" t="inlineStr"/>
       <c r="AA15" s="3" t="inlineStr"/>
+      <c r="AB15" s="3" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
@@ -2228,6 +2263,9 @@
       <c r="AA16" s="2" t="n">
         <v>0.1516316</v>
       </c>
+      <c r="AB16" s="2" t="n">
+        <v>-10.13073792006415</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
@@ -2341,6 +2379,9 @@
       <c r="AA17" s="3" t="n">
         <v>6.594931399523582</v>
       </c>
+      <c r="AB17" s="3" t="n">
+        <v>11.27275075548432</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
@@ -2450,6 +2491,7 @@
       </c>
       <c r="Z18" s="3" t="inlineStr"/>
       <c r="AA18" s="3" t="inlineStr"/>
+      <c r="AB18" s="3" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
@@ -2559,6 +2601,7 @@
       </c>
       <c r="Z19" s="3" t="inlineStr"/>
       <c r="AA19" s="3" t="inlineStr"/>
+      <c r="AB19" s="3" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
@@ -2668,6 +2711,7 @@
       </c>
       <c r="Z20" s="3" t="inlineStr"/>
       <c r="AA20" s="3" t="inlineStr"/>
+      <c r="AB20" s="3" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
@@ -2777,6 +2821,7 @@
       </c>
       <c r="Z21" s="3" t="inlineStr"/>
       <c r="AA21" s="3" t="inlineStr"/>
+      <c r="AB21" s="3" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
@@ -2886,6 +2931,7 @@
       </c>
       <c r="Z22" s="3" t="inlineStr"/>
       <c r="AA22" s="3" t="inlineStr"/>
+      <c r="AB22" s="3" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -2993,8 +3039,15 @@
       <c r="Y23" s="2" t="n">
         <v>-9.470000000000001</v>
       </c>
-      <c r="Z23" s="2" t="inlineStr"/>
-      <c r="AA23" s="2" t="inlineStr"/>
+      <c r="Z23" s="2" t="n">
+        <v>0.08673139999999999</v>
+      </c>
+      <c r="AA23" s="2" t="n">
+        <v>0.09739480000000002</v>
+      </c>
+      <c r="AB23" s="2" t="n">
+        <v>-10.94863380796514</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
@@ -3102,8 +3155,15 @@
       <c r="Y24" s="3" t="n">
         <v>-12.28</v>
       </c>
-      <c r="Z24" s="3" t="inlineStr"/>
-      <c r="AA24" s="3" t="inlineStr"/>
+      <c r="Z24" s="3" t="n">
+        <v>11.52984962770116</v>
+      </c>
+      <c r="AA24" s="3" t="n">
+        <v>10.26748861335513</v>
+      </c>
+      <c r="AB24" s="3" t="n">
+        <v>12.2947398520029</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
@@ -3213,6 +3273,7 @@
       </c>
       <c r="Z25" s="3" t="inlineStr"/>
       <c r="AA25" s="3" t="inlineStr"/>
+      <c r="AB25" s="3" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
@@ -3322,6 +3383,7 @@
       </c>
       <c r="Z26" s="3" t="inlineStr"/>
       <c r="AA26" s="3" t="inlineStr"/>
+      <c r="AB26" s="3" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
@@ -3431,6 +3493,7 @@
       </c>
       <c r="Z27" s="3" t="inlineStr"/>
       <c r="AA27" s="3" t="inlineStr"/>
+      <c r="AB27" s="3" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
@@ -3540,6 +3603,7 @@
       </c>
       <c r="Z28" s="3" t="inlineStr"/>
       <c r="AA28" s="3" t="inlineStr"/>
+      <c r="AB28" s="3" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
@@ -3649,6 +3713,7 @@
       </c>
       <c r="Z29" s="3" t="inlineStr"/>
       <c r="AA29" s="3" t="inlineStr"/>
+      <c r="AB29" s="3" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
@@ -3756,8 +3821,15 @@
       <c r="Y30" s="2" t="n">
         <v>-3.169</v>
       </c>
-      <c r="Z30" s="2" t="inlineStr"/>
-      <c r="AA30" s="2" t="inlineStr"/>
+      <c r="Z30" s="2" t="n">
+        <v>0.259733</v>
+      </c>
+      <c r="AA30" s="2" t="n">
+        <v>0.283546</v>
+      </c>
+      <c r="AB30" s="2" t="n">
+        <v>-8.398284581690438</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
@@ -3865,8 +3937,15 @@
       <c r="Y31" s="3" t="n">
         <v>-11.17</v>
       </c>
-      <c r="Z31" s="3" t="inlineStr"/>
-      <c r="AA31" s="3" t="inlineStr"/>
+      <c r="Z31" s="3" t="n">
+        <v>3.850107610507713</v>
+      </c>
+      <c r="AA31" s="3" t="n">
+        <v>3.526764616675953</v>
+      </c>
+      <c r="AB31" s="3" t="n">
+        <v>9.168261252902004</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
@@ -3976,6 +4055,7 @@
       </c>
       <c r="Z32" s="3" t="inlineStr"/>
       <c r="AA32" s="3" t="inlineStr"/>
+      <c r="AB32" s="3" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
@@ -4085,6 +4165,7 @@
       </c>
       <c r="Z33" s="3" t="inlineStr"/>
       <c r="AA33" s="3" t="inlineStr"/>
+      <c r="AB33" s="3" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
@@ -4194,6 +4275,7 @@
       </c>
       <c r="Z34" s="3" t="inlineStr"/>
       <c r="AA34" s="3" t="inlineStr"/>
+      <c r="AB34" s="3" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
@@ -4303,6 +4385,7 @@
       </c>
       <c r="Z35" s="3" t="inlineStr"/>
       <c r="AA35" s="3" t="inlineStr"/>
+      <c r="AB35" s="3" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
@@ -4412,6 +4495,7 @@
       </c>
       <c r="Z36" s="3" t="inlineStr"/>
       <c r="AA36" s="3" t="inlineStr"/>
+      <c r="AB36" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>